<commit_message>
google ai api pool
</commit_message>
<xml_diff>
--- a/batch/tasks_setting.xlsx
+++ b/batch/tasks_setting.xlsx
@@ -1076,7 +1076,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Error: Unhandled exception - Number of videos found is not unique. Please check. Number of videos found: 2</t>
+          <t>Error: 📝 Summarizing and translating - Still failed after 3 attempts: Error code: 504 - {'code': 50501, 'message': 'Model service timeout. Please try again later.', 'data': None}</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Error: Unhandled exception - Number of videos found is not unique. Please check. Number of videos found: 3</t>
+          <t>Error: 🎙️ Transcribing with Whisper - Expecting value: line 1 column 1 (char 0)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Error: Unhandled exception - Number of videos found is not unique. Please check. Number of videos found: 3</t>
+          <t>Error: 🗣️ Generating audio - Command '['ffmpeg', '-i', 'output/audio/tmp/337_0_temp.wav', '-filter:a', 'atempo=-0.007', '-y', 'output/audio/segs/337_0.wav']' returned non-zero exit status 222.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -1164,7 +1164,11 @@
       <c r="D40" t="n">
         <v>1</v>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Error: 🗣️ Generating audio - Command '['ffmpeg', '-i', 'output/audio/tmp/337_0_temp.wav', '-filter:a', 'atempo=-0.007', '-y', 'output/audio/segs/337_0.wav']' returned non-zero exit status 222.</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">

</xml_diff>

<commit_message>
fix wisper audio split issue
</commit_message>
<xml_diff>
--- a/batch/tasks_setting.xlsx
+++ b/batch/tasks_setting.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Error: 📝 Summarizing and translating - Still failed after 3 attempts: Error code: 504 - {'code': 50501, 'message': 'Model service timeout. Please try again later.', 'data': None}</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Error: 🎙️ Transcribing with Whisper - Expecting value: line 1 column 1 (char 0)</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Error: 🗣️ Generating audio - Command '['ffmpeg', '-i', 'output/audio/tmp/337_0_temp.wav', '-filter:a', 'atempo=-0.007', '-y', 'output/audio/segs/337_0.wav']' returned non-zero exit status 222.</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Error: 🗣️ Generating audio - Command '['ffmpeg', '-i', 'output/audio/tmp/337_0_temp.wav', '-filter:a', 'atempo=-0.007', '-y', 'output/audio/segs/337_0.wav']' returned non-zero exit status 222.</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -1182,7 +1182,11 @@
       <c r="D41" t="n">
         <v>1</v>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -1196,7 +1200,11 @@
       <c r="D42" t="n">
         <v>1</v>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
@@ -1210,7 +1218,11 @@
       <c r="D43" t="n">
         <v>1</v>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
@@ -1224,7 +1236,11 @@
       <c r="D44" t="n">
         <v>1</v>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
@@ -1238,7 +1254,11 @@
       <c r="D45" t="n">
         <v>1</v>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
@@ -1252,7 +1272,11 @@
       <c r="D46" t="n">
         <v>1</v>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
@@ -1266,7 +1290,11 @@
       <c r="D47" t="n">
         <v>1</v>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
@@ -1280,7 +1308,11 @@
       <c r="D48" t="n">
         <v>1</v>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -1294,8 +1326,342 @@
       <c r="D49" t="n">
         <v>1</v>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=70y6hMyRZfQ&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=25&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=eHiqrRloaGc&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=28&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Kp61Z_TKJFk&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=31&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=p6WfKfrLhdQ&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=34&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=pswBnrF5Z5Y&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=37&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=PUscmv4YqMU&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=42&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=viY5RFtIjo0&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=46&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Z4EpFOmyf_g&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=49&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=K1ipCo_KCdI&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=55&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=gunJ_nYCe4k&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=59&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ZYfAO1VJ0r8&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=63&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=5-Hi6SXvrgU&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=67&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=NALYks6kRM0&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=71&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=AFvQjxICn3E&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=75&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=aNPW8VA8wBo&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=79&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=F5jyrHQff9w&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=82&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=hKVpdmjvGRA&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=86&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=8OLHwss-D20&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=90&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=eSs9wOgLTWE&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=94&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=7d5Vs-ha1XU&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=97&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QFkk5cN91B0&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=100&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=gQQG8KK5gQU&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=105&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=2uj0bE7yQhw&amp;list=PLipLTGfSGq9EZDjrAi7VnUf7loK35l19x&amp;index=109&amp;pp=iAQB</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>